<commit_message>
fixed jaarselectie bij totaal overzicht uren
</commit_message>
<xml_diff>
--- a/UrenRegistratieQien/Downloads/25.xlsx
+++ b/UrenRegistratieQien/Downloads/25.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="50">
   <si>
     <t xml:space="preserve">Datum</t>
   </si>
@@ -44,19 +44,25 @@
     <t xml:space="preserve">1/Januari/2020</t>
   </si>
   <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drukke dag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2/Januari/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3/Januari/2020</t>
+  </si>
+  <si>
     <t xml:space="preserve">7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drukke dag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2/Januari/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3/Januari/2020</t>
   </si>
   <si>
     <t xml:space="preserve">4/Januari/2020</t>
@@ -268,7 +274,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -292,10 +298,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -319,10 +325,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -346,13 +352,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -361,7 +367,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -373,7 +379,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -385,7 +391,7 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -400,7 +406,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -427,10 +433,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -454,10 +460,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -481,10 +487,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -508,10 +514,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -523,7 +529,7 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
@@ -535,7 +541,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -547,7 +553,7 @@
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F13" t="s">
         <v>11</v>
@@ -562,7 +568,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -589,10 +595,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
@@ -616,10 +622,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -643,10 +649,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
@@ -670,10 +676,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -697,10 +703,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
@@ -724,10 +730,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -751,7 +757,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
@@ -778,7 +784,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
@@ -805,7 +811,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
@@ -832,13 +838,13 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -850,7 +856,7 @@
         <v>11</v>
       </c>
       <c r="G24" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H24" t="s">
         <v>11</v>
@@ -859,10 +865,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -877,7 +883,7 @@
         <v>11</v>
       </c>
       <c r="G25" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H25" t="s">
         <v>11</v>
@@ -886,10 +892,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
@@ -904,7 +910,7 @@
         <v>11</v>
       </c>
       <c r="G26" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H26" t="s">
         <v>11</v>
@@ -913,10 +919,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
@@ -931,7 +937,7 @@
         <v>11</v>
       </c>
       <c r="G27" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H27" t="s">
         <v>11</v>
@@ -940,7 +946,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
         <v>11</v>
@@ -967,7 +973,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
@@ -994,7 +1000,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
@@ -1021,7 +1027,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
@@ -1048,7 +1054,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>

</xml_diff>